<commit_message>
Add new results of basic experiment
</commit_message>
<xml_diff>
--- a/results/basic_metrics_runtimes/TPE_tuning_150_50_trees/results_accuracy_12_datasets_TPE_150_50_trees.xlsx
+++ b/results/basic_metrics_runtimes/TPE_tuning_150_50_trees/results_accuracy_12_datasets_TPE_150_50_trees.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p\Documents\M\2 stopień\masters thesis\boost\results\basic_metrics_runtimes\TPE_tuning_150_50_trees\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA83C69-F91B-42BA-AB27-271DC9D14A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9223806-766B-452F-999A-3CD0AADDCAD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -126,12 +126,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -2328,172 +2327,172 @@
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A112" s="2">
+      <c r="A112">
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="B112">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="C112">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="D112">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="E112" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>0.83</v>
+      </c>
+      <c r="B113">
+        <v>0.82799999999999996</v>
+      </c>
+      <c r="C113">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="D113">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="E113" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="B114">
+        <v>0.83</v>
+      </c>
+      <c r="C114">
+        <v>0.84299999999999997</v>
+      </c>
+      <c r="D114">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="E114" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="B115">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="C115">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="D115">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="E115" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <v>0.83</v>
+      </c>
+      <c r="B116">
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="C116">
+        <v>0.82599999999999996</v>
+      </c>
+      <c r="D116">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="E116" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="B117">
+        <v>0.83</v>
+      </c>
+      <c r="C117">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="D117">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="E117" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A118">
         <v>0.79300000000000004</v>
       </c>
-      <c r="B112" s="2">
-        <v>0.80700000000000005</v>
-      </c>
-      <c r="C112" s="2">
-        <v>0.81499999999999995</v>
-      </c>
-      <c r="D112" s="2">
-        <v>0.71399999999999997</v>
-      </c>
-      <c r="E112" s="2" t="s">
+      <c r="B118">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="C118">
+        <v>0.80400000000000005</v>
+      </c>
+      <c r="D118">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="E118" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A113" s="2">
-        <v>0.81599999999999995</v>
-      </c>
-      <c r="B113" s="2">
-        <v>0.82799999999999996</v>
-      </c>
-      <c r="C113" s="2">
-        <v>0.83099999999999996</v>
-      </c>
-      <c r="D113" s="2">
-        <v>0.75700000000000001</v>
-      </c>
-      <c r="E113" s="2" t="s">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="B119">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="C119">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="D119">
+        <v>0.753</v>
+      </c>
+      <c r="E119" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A114" s="2">
-        <v>0.83899999999999997</v>
-      </c>
-      <c r="B114" s="2">
-        <v>0.83</v>
-      </c>
-      <c r="C114" s="2">
-        <v>0.84299999999999997</v>
-      </c>
-      <c r="D114" s="2">
-        <v>0.75800000000000001</v>
-      </c>
-      <c r="E114" s="2" t="s">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="B120">
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="C120">
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="D120">
+        <v>0.76900000000000002</v>
+      </c>
+      <c r="E120" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A115" s="2">
-        <v>0.81499999999999995</v>
-      </c>
-      <c r="B115" s="2">
-        <v>0.81399999999999995</v>
-      </c>
-      <c r="C115" s="2">
-        <v>0.83499999999999996</v>
-      </c>
-      <c r="D115" s="2">
-        <v>0.75600000000000001</v>
-      </c>
-      <c r="E115" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A116" s="2">
-        <v>0.81</v>
-      </c>
-      <c r="B116" s="2">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="B121">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="C121">
         <v>0.81299999999999994</v>
       </c>
-      <c r="C116" s="2">
-        <v>0.82599999999999996</v>
-      </c>
-      <c r="D116" s="2">
-        <v>0.77400000000000002</v>
-      </c>
-      <c r="E116" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A117" s="2">
-        <v>0.82499999999999996</v>
-      </c>
-      <c r="B117" s="2">
-        <v>0.83</v>
-      </c>
-      <c r="C117" s="2">
-        <v>0.82099999999999995</v>
-      </c>
-      <c r="D117" s="2">
-        <v>0.76200000000000001</v>
-      </c>
-      <c r="E117" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A118" s="2">
-        <v>0.79600000000000004</v>
-      </c>
-      <c r="B118" s="2">
-        <v>0.78800000000000003</v>
-      </c>
-      <c r="C118" s="2">
-        <v>0.80400000000000005</v>
-      </c>
-      <c r="D118" s="2">
-        <v>0.72499999999999998</v>
-      </c>
-      <c r="E118" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A119" s="2">
-        <v>0.79400000000000004</v>
-      </c>
-      <c r="B119" s="2">
-        <v>0.81899999999999995</v>
-      </c>
-      <c r="C119" s="2">
-        <v>0.82499999999999996</v>
-      </c>
-      <c r="D119" s="2">
-        <v>0.753</v>
-      </c>
-      <c r="E119" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A120" s="2">
-        <v>0.82399999999999995</v>
-      </c>
-      <c r="B120" s="2">
-        <v>0.81299999999999994</v>
-      </c>
-      <c r="C120" s="2">
-        <v>0.84099999999999997</v>
-      </c>
-      <c r="D120" s="2">
-        <v>0.76900000000000002</v>
-      </c>
-      <c r="E120" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A121" s="2">
-        <v>0.80800000000000005</v>
-      </c>
-      <c r="B121" s="2">
-        <v>0.81699999999999995</v>
-      </c>
-      <c r="C121" s="2">
-        <v>0.81299999999999994</v>
-      </c>
-      <c r="D121" s="2">
+      <c r="D121">
         <v>0.76600000000000001</v>
       </c>
-      <c r="E121" s="2" t="s">
+      <c r="E121" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>